<commit_message>
Agregar codigo y agregar estimacion Bernal
</commit_message>
<xml_diff>
--- a/Data/UDEP_1991-2019.xlsx
+++ b/Data/UDEP_1991-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Tesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B162687F-6D33-4178-A4F8-46EE45A05971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDE253D-C42F-49F4-8D53-2FA7838E3A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1A1A1C07-F415-4062-AF83-746E68B08CEC}"/>
   </bookViews>
@@ -8109,8 +8109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1584AD87-B3AE-4A30-BA44-91C91E8959D2}">
   <dimension ref="A3:E603"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A584" workbookViewId="0">
-      <selection activeCell="G597" sqref="G597"/>
+    <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
+      <selection activeCell="E518" sqref="E518"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14418,6 +14418,9 @@
       <c r="C523" s="10">
         <v>2.6</v>
       </c>
+      <c r="D523" s="30">
+        <v>34.6</v>
+      </c>
       <c r="E523" s="30">
         <v>19.5</v>
       </c>
@@ -14432,6 +14435,9 @@
       <c r="C524" s="10">
         <v>0.6</v>
       </c>
+      <c r="D524" s="30">
+        <v>33.200000000000003</v>
+      </c>
       <c r="E524" s="30">
         <v>21.2</v>
       </c>
@@ -14446,6 +14452,9 @@
       <c r="C525" s="11">
         <v>0</v>
       </c>
+      <c r="D525" s="30">
+        <v>33</v>
+      </c>
       <c r="E525" s="30">
         <v>19.100000000000001</v>
       </c>
@@ -14460,6 +14469,9 @@
       <c r="C526" s="11">
         <v>0</v>
       </c>
+      <c r="D526" s="30">
+        <v>31</v>
+      </c>
       <c r="E526" s="30">
         <v>15.8</v>
       </c>
@@ -14474,6 +14486,9 @@
       <c r="C527" s="11">
         <v>0</v>
       </c>
+      <c r="D527" s="30">
+        <v>31.9</v>
+      </c>
       <c r="E527" s="30">
         <v>15.7</v>
       </c>
@@ -14488,6 +14503,9 @@
       <c r="C528" s="11">
         <v>0</v>
       </c>
+      <c r="D528" s="30">
+        <v>32.200000000000003</v>
+      </c>
       <c r="E528" s="30">
         <v>16.600000000000001</v>
       </c>
@@ -14502,6 +14520,9 @@
       <c r="C529" s="10">
         <v>1.9</v>
       </c>
+      <c r="D529" s="30">
+        <v>32.4</v>
+      </c>
       <c r="E529" s="30">
         <v>16.600000000000001</v>
       </c>
@@ -14516,6 +14537,9 @@
       <c r="C530" s="11">
         <v>0</v>
       </c>
+      <c r="D530" s="30">
+        <v>32.200000000000003</v>
+      </c>
       <c r="E530" s="30">
         <v>17.600000000000001</v>
       </c>
@@ -14529,6 +14553,9 @@
       </c>
       <c r="C531" s="10">
         <v>1.1000000000000001</v>
+      </c>
+      <c r="D531" s="30">
+        <v>33.4</v>
       </c>
       <c r="E531" s="30">
         <v>18.7</v>

</xml_diff>